<commit_message>
Guess what this is
</commit_message>
<xml_diff>
--- a/Demo/item.xlsx
+++ b/Demo/item.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3120" yWindow="1755" windowWidth="21600" windowHeight="11835" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3120" yWindow="1755" windowWidth="21600" windowHeight="11835" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" state="visible" r:id="rId1"/>
@@ -424,10 +424,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -436,41 +436,6 @@
       <c r="A1" t="inlineStr">
         <is>
           <t>지도</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>손전등</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>창고열쇠</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>보안키</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>연구일지</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>오징어 맛살</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>똥</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>500원</t>
         </is>
       </c>
     </row>
@@ -493,10 +458,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -522,6 +487,11 @@
           <t>설명(안적어도됨)</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>배고픔 회복량</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -693,6 +663,40 @@
         <v>2</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>카드키</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>10</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>보안실, 창고, 관리실 등에서 사용 가능</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>빵</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>배고픔 20 회복</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -705,10 +709,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
@@ -763,6 +767,11 @@
       <c r="A4" t="inlineStr">
         <is>
           <t>상자2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>빵</t>
         </is>
       </c>
     </row>
@@ -801,7 +810,7 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>